<commit_message>
Derniers resultats, avec 100M et 50M d'iterations. Les fichier choisit commencent par des majuscules JEU_BJ_CLASSIQUE_mypolicy_IAvsBank_asymetrique_100M_v2 et JEU_SYM_mypolicy_IAvsIA_100M_v4
</commit_message>
<xml_diff>
--- a/mypolicy_IAvsIA_100M_v2.xlsx
+++ b/mypolicy_IAvsIA_100M_v2.xlsx
@@ -620,8 +620,8 @@
       <c r="I5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="J5" s="3" t="n">
-        <v>0</v>
+      <c r="J5" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="K5" s="3" t="n">
         <v>0</v>
@@ -649,8 +649,8 @@
       <c r="B6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>1</v>
+      <c r="C6" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="D6" s="4" t="n">
         <v>2</v>
@@ -720,8 +720,8 @@
       <c r="I7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="J7" s="3" t="n">
-        <v>0</v>
+      <c r="J7" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="K7" s="3" t="n">
         <v>0</v>
@@ -746,11 +746,11 @@
       <c r="A8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>1</v>
+      <c r="B8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="D8" s="4" t="n">
         <v>2</v>
@@ -767,8 +767,8 @@
       <c r="H8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="3" t="n">
-        <v>0</v>
+      <c r="I8" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J8" s="3" t="n">
         <v>0</v>
@@ -799,8 +799,8 @@
       <c r="B9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>1</v>
+      <c r="C9" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>1</v>
@@ -855,8 +855,8 @@
       <c r="D10" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="2" t="n">
-        <v>1</v>
+      <c r="E10" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>1</v>
@@ -902,8 +902,8 @@
       <c r="C11" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D11" s="4" t="n">
-        <v>2</v>
+      <c r="D11" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="E11" s="4" t="n">
         <v>2</v>
@@ -973,8 +973,8 @@
       <c r="J12" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="K12" s="3" t="n">
-        <v>0</v>
+      <c r="K12" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="L12" s="3" t="n">
         <v>0</v>
@@ -1023,8 +1023,8 @@
       <c r="J13" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="K13" s="3" t="n">
-        <v>0</v>
+      <c r="K13" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="L13" s="3" t="n">
         <v>0</v>
@@ -1134,8 +1134,8 @@
       <c r="F19" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G19" s="4" t="n">
-        <v>2</v>
+      <c r="G19" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="H19" s="3" t="n">
         <v>0</v>
@@ -1195,11 +1195,11 @@
       <c r="E21" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F21" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="4" t="n">
-        <v>2</v>
+      <c r="F21" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="H21" s="3" t="n">
         <v>0</v>
@@ -1215,8 +1215,8 @@
       <c r="A22" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B22" s="4" t="n">
-        <v>2</v>
+      <c r="B22" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>1</v>
@@ -1227,8 +1227,8 @@
       <c r="E22" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F22" s="4" t="n">
-        <v>2</v>
+      <c r="F22" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="G22" s="3" t="n">
         <v>0</v>
@@ -1256,11 +1256,11 @@
       <c r="D23" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E23" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2" t="n">
-        <v>1</v>
+      <c r="E23" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="G23" s="3" t="n">
         <v>0</v>
@@ -1291,8 +1291,8 @@
       <c r="E24" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F24" s="4" t="n">
-        <v>2</v>
+      <c r="F24" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="G24" s="3" t="n">
         <v>0</v>
@@ -1390,8 +1390,8 @@
       <c r="F27" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G27" s="3" t="n">
-        <v>0</v>
+      <c r="G27" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="H27" s="3" t="n">
         <v>0</v>
@@ -1504,8 +1504,8 @@
       <c r="G33" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H33" s="5" t="n">
-        <v>3</v>
+      <c r="H33" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="I33" s="5" t="n">
         <v>3</v>
@@ -1521,8 +1521,8 @@
       <c r="A34" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="n">
-        <v>3</v>
+      <c r="B34" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>1</v>
@@ -1533,14 +1533,14 @@
       <c r="E34" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F34" s="2" t="n">
-        <v>1</v>
+      <c r="F34" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="G34" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H34" s="4" t="n">
-        <v>2</v>
+      <c r="H34" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="I34" s="5" t="n">
         <v>3</v>
@@ -1556,8 +1556,8 @@
       <c r="A35" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B35" s="2" t="n">
-        <v>1</v>
+      <c r="B35" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>1</v>
@@ -1591,14 +1591,14 @@
       <c r="A36" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B36" s="5" t="n">
-        <v>3</v>
+      <c r="B36" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D36" s="5" t="n">
-        <v>3</v>
+      <c r="D36" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>1</v>
@@ -1606,8 +1606,8 @@
       <c r="F36" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G36" s="5" t="n">
-        <v>3</v>
+      <c r="G36" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="H36" s="5" t="n">
         <v>3</v>
@@ -1615,8 +1615,8 @@
       <c r="I36" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="J36" s="5" t="n">
-        <v>3</v>
+      <c r="J36" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="K36" s="3" t="n">
         <v>0</v>
@@ -1632,14 +1632,14 @@
       <c r="C37" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D37" s="2" t="n">
-        <v>1</v>
+      <c r="D37" s="5" t="n">
+        <v>3</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F37" s="2" t="n">
-        <v>1</v>
+      <c r="F37" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="G37" s="2" t="n">
         <v>1</v>
@@ -1661,23 +1661,23 @@
       <c r="A38" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B38" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C38" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D38" s="5" t="n">
-        <v>3</v>
+      <c r="B38" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="E38" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F38" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G38" s="5" t="n">
-        <v>3</v>
+      <c r="F38" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G38" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="H38" s="5" t="n">
         <v>3</v>
@@ -1702,8 +1702,8 @@
       <c r="C39" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D39" s="5" t="n">
-        <v>3</v>
+      <c r="D39" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="E39" s="2" t="n">
         <v>1</v>
@@ -1743,8 +1743,8 @@
       <c r="E40" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F40" s="4" t="n">
-        <v>2</v>
+      <c r="F40" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="G40" s="2" t="n">
         <v>1</v>
@@ -1752,8 +1752,8 @@
       <c r="H40" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I40" s="3" t="n">
-        <v>0</v>
+      <c r="I40" s="5" t="n">
+        <v>3</v>
       </c>
       <c r="J40" s="5" t="n">
         <v>3</v>

</xml_diff>